<commit_message>
Update Nome do Arquivo e Atualização da Base
</commit_message>
<xml_diff>
--- a/Teste.xlsx
+++ b/Teste.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">Teste 1</t>
   </si>
@@ -59,6 +59,39 @@
   </si>
   <si>
     <t xml:space="preserve">g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">j</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r</t>
   </si>
 </sst>
 </file>
@@ -170,10 +203,10 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
@@ -202,58 +235,123 @@
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2" s="0" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
+      <c r="A3" s="0" t="s">
+        <v>6</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="C3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="0" t="n">
         <v>8</v>
       </c>
+      <c r="C4" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>4</v>
+      <c r="A5" s="0" t="s">
+        <v>12</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>6</v>
+      <c r="A7" s="0" t="s">
+        <v>18</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
+        <v>19</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>